<commit_message>
modified:   MonteCarlo_Sim.py 	modified:   Outputs/MonteCarlo_sim_inputs.xlsx 	modified:   Outputs/MonteCarlo_sim_outputs.xlsx 	modified:   Outputs/WindData/Final_Wind.json 	deleted:    Outputs/WindData/Winddata2016.json 	deleted:    Outputs/WindData/Winddata2017.json 	deleted:    Outputs/WindData/Winddata2019.json 	new file:   Outputs/WindData/Winddata2020.json 	modified:   Wind_Analysis.py 	modified:   Wind_Data.py
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_inputs.xlsx
+++ b/Outputs/MonteCarlo_sim_inputs.xlsx
@@ -463,10 +463,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.0789137132821822</v>
+        <v>0.07842550411241363</v>
       </c>
       <c r="C2">
-        <v>0.07868099934256596</v>
+        <v>0.07857737532631999</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -474,10 +474,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>25.84973899425027</v>
+        <v>25.85035106517594</v>
       </c>
       <c r="C3">
-        <v>25.85183186790679</v>
+        <v>25.84855247754756</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -485,10 +485,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>151.6998082772819</v>
+        <v>151.7002690322068</v>
       </c>
       <c r="C4">
-        <v>151.6998386201667</v>
+        <v>151.7001064987981</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -496,10 +496,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1859355621718312</v>
+        <v>0.1861700271909474</v>
       </c>
       <c r="C5">
-        <v>0.18580592255242</v>
+        <v>0.1861838425959638</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -507,10 +507,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.260004129438739</v>
+        <v>2.260007709475259</v>
       </c>
       <c r="C6">
-        <v>2.259996354509955</v>
+        <v>2.260014913317138</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -518,10 +518,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3.459688471232211</v>
+        <v>3.453383257753605</v>
       </c>
       <c r="C7">
-        <v>3.45080396636782</v>
+        <v>3.452593341633722</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -529,10 +529,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>28.34748166839677</v>
+        <v>28.34464335168526</v>
       </c>
       <c r="C8">
-        <v>28.34470187142677</v>
+        <v>28.34602275907135</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -540,10 +540,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.016378560511173</v>
+        <v>0.9688101420794846</v>
       </c>
       <c r="C9">
-        <v>0.9841998007608717</v>
+        <v>0.9942548566434352</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -551,10 +551,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.053429780850328</v>
+        <v>0.9457490135755082</v>
       </c>
       <c r="C10">
-        <v>0.9630437522993498</v>
+        <v>1.001193114688219</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -562,10 +562,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2.147594630881775</v>
+        <v>2.148125598797401</v>
       </c>
       <c r="C11">
-        <v>2.148155995024835</v>
+        <v>2.147445049741169</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -573,10 +573,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.9139800805208471</v>
+        <v>0.9138891466183333</v>
       </c>
       <c r="C12">
-        <v>0.9137761846411234</v>
+        <v>0.9137399636249539</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -584,10 +584,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.07806940196443339</v>
+        <v>0.07758314689643474</v>
       </c>
       <c r="C13">
-        <v>0.07780869144750975</v>
+        <v>0.07822793580709947</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -617,10 +617,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5593591861331478</v>
+        <v>0.5611242618245873</v>
       </c>
       <c r="C16">
-        <v>0.5554508378094879</v>
+        <v>0.5576612645469076</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -628,10 +628,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.1775448393396856</v>
+        <v>0.1806608123700188</v>
       </c>
       <c r="C17">
-        <v>0.1777172363942013</v>
+        <v>0.1803985511818771</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -639,10 +639,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.1249704110309329</v>
+        <v>0.1270626374706491</v>
       </c>
       <c r="C18">
-        <v>0.1273668682629146</v>
+        <v>0.1269700044132066</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -650,10 +650,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>5.109246515736505</v>
+        <v>5.108799270348942</v>
       </c>
       <c r="C19">
-        <v>5.107562565383643</v>
+        <v>5.109979331599349</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -661,10 +661,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.001087139746332026</v>
+        <v>0.0001810799230792221</v>
       </c>
       <c r="C20">
-        <v>-0.0002072084976323606</v>
+        <v>0.00122143856021752</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -672,10 +672,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.4699693719456701</v>
+        <v>0.4683879945133046</v>
       </c>
       <c r="C21">
-        <v>0.4672571729623264</v>
+        <v>0.4699436266384943</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -683,10 +683,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>28.3524248179841</v>
+        <v>28.35029177129032</v>
       </c>
       <c r="C22">
-        <v>28.35083228300352</v>
+        <v>28.35020138343259</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -694,10 +694,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>29.29980754823187</v>
+        <v>29.30002606027189</v>
       </c>
       <c r="C23">
-        <v>29.30019617255651</v>
+        <v>29.29969264114588</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -705,10 +705,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.08189342097516634</v>
+        <v>0.08195326951965419</v>
       </c>
       <c r="C24">
-        <v>0.08173283511072502</v>
+        <v>0.08187307750006102</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -716,10 +716,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.455241887514029</v>
+        <v>0.4545261387909518</v>
       </c>
       <c r="C25">
-        <v>0.4544256066037909</v>
+        <v>0.4545223257423662</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -727,10 +727,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1.706341867730033</v>
+        <v>1.707130551153438</v>
       </c>
       <c r="C26">
-        <v>1.706039511915585</v>
+        <v>1.70751982552766</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -738,10 +738,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3.595228705949467</v>
+        <v>3.596326654411414</v>
       </c>
       <c r="C27">
-        <v>3.596693457007799</v>
+        <v>3.593880411960965</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -749,10 +749,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>12.0658475568507</v>
+        <v>12.06509528600064</v>
       </c>
       <c r="C28">
-        <v>12.0663525364599</v>
+        <v>12.0670489237679</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -760,10 +760,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>33.07129975607472</v>
+        <v>33.02626999186418</v>
       </c>
       <c r="C29">
-        <v>33.36857227250622</v>
+        <v>34.04164878115266</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -771,10 +771,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>73818.60722851334</v>
+        <v>73848.18772607749</v>
       </c>
       <c r="C30">
-        <v>73823.86565015042</v>
+        <v>73869.78685537845</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -782,10 +782,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6.094279056683153</v>
+        <v>6.094545837876081</v>
       </c>
       <c r="C31">
-        <v>6.094083724939274</v>
+        <v>6.094775018940848</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -793,10 +793,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>88.47128878314591</v>
+        <v>87.92925601430773</v>
       </c>
       <c r="C32">
-        <v>87.91445493763064</v>
+        <v>87.79056250758926</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -804,10 +804,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>-9.947013548357424E-05</v>
+        <v>-0.0002544782442354753</v>
       </c>
       <c r="C33">
-        <v>9.355540872633562E-05</v>
+        <v>-0.0007370429121234176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   MonteCarlo_Sim.py 	modified:   Outputs/MonteCarlo_sim_inputs.xlsx 	modified:   Outputs/MonteCarlo_sim_outputs.xlsx 	modified:   Outputs/WindData/Final_Wind.json
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_inputs.xlsx
+++ b/Outputs/MonteCarlo_sim_inputs.xlsx
@@ -463,10 +463,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.07842550411241363</v>
+        <v>0.0785058923029907</v>
       </c>
       <c r="C2">
-        <v>0.07857737532631999</v>
+        <v>0.07879932249964856</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -474,10 +474,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>25.85035106517594</v>
+        <v>25.8507665079589</v>
       </c>
       <c r="C3">
-        <v>25.84855247754756</v>
+        <v>25.84962391117613</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -485,10 +485,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>151.7002690322068</v>
+        <v>151.7000171572285</v>
       </c>
       <c r="C4">
-        <v>151.7001064987981</v>
+        <v>151.6998888889504</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -496,10 +496,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1861700271909474</v>
+        <v>0.1860813878608437</v>
       </c>
       <c r="C5">
-        <v>0.1861838425959638</v>
+        <v>0.1863763212861354</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -507,10 +507,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.260007709475259</v>
+        <v>2.2599826594633</v>
       </c>
       <c r="C6">
-        <v>2.260014913317138</v>
+        <v>2.260010699463755</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -518,10 +518,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3.453383257753605</v>
+        <v>3.446411539251389</v>
       </c>
       <c r="C7">
-        <v>3.452593341633722</v>
+        <v>3.460343982477563</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -529,10 +529,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>28.34464335168526</v>
+        <v>28.34446575857872</v>
       </c>
       <c r="C8">
-        <v>28.34602275907135</v>
+        <v>28.35036153016067</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -540,10 +540,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.9688101420794846</v>
+        <v>0.9985560960564827</v>
       </c>
       <c r="C9">
-        <v>0.9942548566434352</v>
+        <v>1.001990562274371</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -551,10 +551,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.9457490135755082</v>
+        <v>1.037626909440452</v>
       </c>
       <c r="C10">
-        <v>1.001193114688219</v>
+        <v>1.02993931306435</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -562,10 +562,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2.148125598797401</v>
+        <v>2.147901651422697</v>
       </c>
       <c r="C11">
-        <v>2.147445049741169</v>
+        <v>2.147528876537519</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -573,10 +573,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.9138891466183333</v>
+        <v>0.9142274572395582</v>
       </c>
       <c r="C12">
-        <v>0.9137399636249539</v>
+        <v>0.9137685644164281</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -584,10 +584,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.07758314689643474</v>
+        <v>0.07819707116398543</v>
       </c>
       <c r="C13">
-        <v>0.07822793580709947</v>
+        <v>0.07852662361418286</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -617,10 +617,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5611242618245873</v>
+        <v>0.5611650814235752</v>
       </c>
       <c r="C16">
-        <v>0.5576612645469076</v>
+        <v>0.5596971337829894</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -628,10 +628,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.1806608123700188</v>
+        <v>0.1760028555701231</v>
       </c>
       <c r="C17">
-        <v>0.1803985511818771</v>
+        <v>0.1782905614990401</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -639,10 +639,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.1270626374706491</v>
+        <v>0.1238448749993802</v>
       </c>
       <c r="C18">
-        <v>0.1269700044132066</v>
+        <v>0.1296115057471527</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -650,10 +650,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>5.108799270348942</v>
+        <v>5.106580426202616</v>
       </c>
       <c r="C19">
-        <v>5.109979331599349</v>
+        <v>5.109398435461945</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -661,10 +661,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.0001810799230792221</v>
+        <v>-0.001518639068848169</v>
       </c>
       <c r="C20">
-        <v>0.00122143856021752</v>
+        <v>0.000425050072496377</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -672,10 +672,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.4683879945133046</v>
+        <v>0.466748659620552</v>
       </c>
       <c r="C21">
-        <v>0.4699436266384943</v>
+        <v>0.4728653484395555</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -683,10 +683,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>28.35029177129032</v>
+        <v>28.35098618505414</v>
       </c>
       <c r="C22">
-        <v>28.35020138343259</v>
+        <v>28.35036122244466</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -694,10 +694,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>29.30002606027189</v>
+        <v>29.29968616819997</v>
       </c>
       <c r="C23">
-        <v>29.29969264114588</v>
+        <v>29.29961077147871</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -705,10 +705,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.08195326951965419</v>
+        <v>0.08170680757140904</v>
       </c>
       <c r="C24">
-        <v>0.08187307750006102</v>
+        <v>0.08153342587004436</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -716,10 +716,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.4545261387909518</v>
+        <v>0.4545569202934908</v>
       </c>
       <c r="C25">
-        <v>0.4545223257423662</v>
+        <v>0.4549170933143945</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -727,10 +727,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1.707130551153438</v>
+        <v>1.706368158243851</v>
       </c>
       <c r="C26">
-        <v>1.70751982552766</v>
+        <v>1.707962202343462</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -738,10 +738,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3.596326654411414</v>
+        <v>3.593914212738785</v>
       </c>
       <c r="C27">
-        <v>3.593880411960965</v>
+        <v>3.593589538502072</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -749,10 +749,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>12.06509528600064</v>
+        <v>12.06594184675126</v>
       </c>
       <c r="C28">
-        <v>12.0670489237679</v>
+        <v>12.06656282398755</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -760,10 +760,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>33.02626999186418</v>
+        <v>33.53453594755665</v>
       </c>
       <c r="C29">
-        <v>34.04164878115266</v>
+        <v>34.14884386934217</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -771,10 +771,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>73848.18772607749</v>
+        <v>73731.47787848058</v>
       </c>
       <c r="C30">
-        <v>73869.78685537845</v>
+        <v>73834.8327812543</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -782,10 +782,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6.094545837876081</v>
+        <v>6.091030113757384</v>
       </c>
       <c r="C31">
-        <v>6.094775018940848</v>
+        <v>6.093138382163727</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -793,10 +793,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>87.92925601430773</v>
+        <v>87.8510884073508</v>
       </c>
       <c r="C32">
-        <v>87.79056250758926</v>
+        <v>88.07489705110397</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -804,10 +804,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>-0.0002544782442354753</v>
+        <v>-0.004194292748618777</v>
       </c>
       <c r="C33">
-        <v>-0.0007370429121234176</v>
+        <v>0.00122776659692803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   Environment_Analysis.py 	modified:   MonteCarlo_Sim.py 	modified:   Outputs/MonteCarlo_sim_inputs.xlsx 	modified:   Outputs/MonteCarlo_sim_outputs.xlsx
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_inputs.xlsx
+++ b/Outputs/MonteCarlo_sim_inputs.xlsx
@@ -441,373 +441,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.0785058923029907</v>
-      </c>
-      <c r="C2">
-        <v>0.07879932249964856</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0.07827832446500971</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>25.8507665079589</v>
-      </c>
-      <c r="C3">
-        <v>25.84962391117613</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>25.85178379958638</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>151.7000171572285</v>
-      </c>
-      <c r="C4">
-        <v>151.6998888889504</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>151.6999506794686</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1860813878608437</v>
-      </c>
-      <c r="C5">
-        <v>0.1863763212861354</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>0.1857483474017147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.2599826594633</v>
-      </c>
-      <c r="C6">
-        <v>2.260010699463755</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>2.259983897591462</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3.446411539251389</v>
-      </c>
-      <c r="C7">
-        <v>3.460343982477563</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>3.45764265479874</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>28.34446575857872</v>
-      </c>
-      <c r="C8">
-        <v>28.35036153016067</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>28.34305588244797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.9985560960564827</v>
-      </c>
-      <c r="C9">
-        <v>1.001990562274371</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>0.996206034574341</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.037626909440452</v>
-      </c>
-      <c r="C10">
-        <v>1.02993931306435</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>1.01519036569497</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2.147901651422697</v>
-      </c>
-      <c r="C11">
-        <v>2.147528876537519</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>2.148267168927628</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.9142274572395582</v>
-      </c>
-      <c r="C12">
-        <v>0.9137685644164281</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>0.9142165883506808</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.07819707116398543</v>
-      </c>
-      <c r="C13">
-        <v>0.07852662361418286</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>0.07829918587575628</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5611650814235752</v>
-      </c>
-      <c r="C16">
-        <v>0.5596971337829894</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>0.5570218339441547</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.1760028555701231</v>
-      </c>
-      <c r="C17">
-        <v>0.1782905614990401</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>0.1789698279133011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.1238448749993802</v>
-      </c>
-      <c r="C18">
-        <v>0.1296115057471527</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>0.1251479657877091</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>5.106580426202616</v>
-      </c>
-      <c r="C19">
-        <v>5.109398435461945</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>5.109587219701581</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-0.001518639068848169</v>
-      </c>
-      <c r="C20">
-        <v>0.000425050072496377</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>0.0117340989070336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.466748659620552</v>
-      </c>
-      <c r="C21">
-        <v>0.4728653484395555</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>0.4685710355772409</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>28.35098618505414</v>
-      </c>
-      <c r="C22">
-        <v>28.35036122244466</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>28.35066765640477</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>29.29968616819997</v>
-      </c>
-      <c r="C23">
-        <v>29.29961077147871</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>29.29956887469033</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.08170680757140904</v>
-      </c>
-      <c r="C24">
-        <v>0.08153342587004436</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>0.08161019259709537</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.4545569202934908</v>
-      </c>
-      <c r="C25">
-        <v>0.4549170933143945</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>0.4545683228568137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1.706368158243851</v>
-      </c>
-      <c r="C26">
-        <v>1.707962202343462</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>1.706235270895844</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3.593914212738785</v>
-      </c>
-      <c r="C27">
-        <v>3.593589538502072</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>3.596233485751527</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>12.06594184675126</v>
-      </c>
-      <c r="C28">
-        <v>12.06656282398755</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>12.06697641810684</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>33.53453594755665</v>
-      </c>
-      <c r="C29">
-        <v>34.14884386934217</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>33.28598225363204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>73731.47787848058</v>
-      </c>
-      <c r="C30">
-        <v>73834.8327812543</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>73817.19939611075</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6.091030113757384</v>
-      </c>
-      <c r="C31">
-        <v>6.093138382163727</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>6.095572920455203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>87.8510884073508</v>
-      </c>
-      <c r="C32">
-        <v>88.07489705110397</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>88.11583049130799</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>-0.004194292748618777</v>
-      </c>
-      <c r="C33">
-        <v>0.00122776659692803</v>
+        <v>50.001183795832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   Outputs/MonteCarlo_sim_inputs.xlsx 	modified:   Outputs/MonteCarlo_sim_outputs.xlsx 	new file:   Outputs/WindData/Winddata2018.json 	new file:   Outputs/WindData/Winddata2020.json 	new file:   Outputs/WindData/Winddata2021.json 	new file:   Outputs/WindData/Winddata2022.json
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_inputs.xlsx
+++ b/Outputs/MonteCarlo_sim_inputs.xlsx
@@ -487,34 +487,34 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.07847760959480324</v>
+        <v>0.07817971878511421</v>
       </c>
       <c r="C2">
-        <v>0.07790990994536423</v>
+        <v>0.0783311784570309</v>
       </c>
       <c r="D2">
-        <v>0.07875983176856631</v>
+        <v>0.07882964468300416</v>
       </c>
       <c r="E2">
-        <v>0.07819140000034416</v>
+        <v>0.07898575576335547</v>
       </c>
       <c r="F2">
-        <v>0.07839303278893857</v>
+        <v>0.0789021773171731</v>
       </c>
       <c r="G2">
-        <v>0.07863902244291529</v>
+        <v>0.07841102167452746</v>
       </c>
       <c r="H2">
-        <v>0.07818730127540516</v>
+        <v>0.07816076904529083</v>
       </c>
       <c r="I2">
-        <v>0.07868990688096771</v>
+        <v>0.07902881765877712</v>
       </c>
       <c r="J2">
-        <v>0.07788522422265916</v>
+        <v>0.07869720463851246</v>
       </c>
       <c r="K2">
-        <v>0.07820416265670023</v>
+        <v>0.07807812593315568</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -522,34 +522,34 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>25.85054037253802</v>
+        <v>25.8498244400453</v>
       </c>
       <c r="C3">
-        <v>25.85044665665422</v>
+        <v>25.84895386915952</v>
       </c>
       <c r="D3">
-        <v>25.85002125762849</v>
+        <v>25.85227483928836</v>
       </c>
       <c r="E3">
-        <v>25.8509305235463</v>
+        <v>25.84965830012807</v>
       </c>
       <c r="F3">
-        <v>25.8526242125383</v>
+        <v>25.84939258695979</v>
       </c>
       <c r="G3">
-        <v>25.85158553590932</v>
+        <v>25.84872764592898</v>
       </c>
       <c r="H3">
-        <v>25.85036745006821</v>
+        <v>25.84893176529916</v>
       </c>
       <c r="I3">
-        <v>25.84965673548191</v>
+        <v>25.84849984402901</v>
       </c>
       <c r="J3">
-        <v>25.84919742887062</v>
+        <v>25.84851247639706</v>
       </c>
       <c r="K3">
-        <v>25.85058005534978</v>
+        <v>25.84989010061628</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -557,34 +557,34 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>151.7000669886547</v>
+        <v>151.6999409060293</v>
       </c>
       <c r="C4">
-        <v>151.6998833150703</v>
+        <v>151.6996680895456</v>
       </c>
       <c r="D4">
-        <v>151.700137911395</v>
+        <v>151.7001258504768</v>
       </c>
       <c r="E4">
-        <v>151.7000046199173</v>
+        <v>151.7002862504015</v>
       </c>
       <c r="F4">
-        <v>151.7000150613295</v>
+        <v>151.6999693512639</v>
       </c>
       <c r="G4">
-        <v>151.7000941281871</v>
+        <v>151.6999072420455</v>
       </c>
       <c r="H4">
-        <v>151.6997241102406</v>
+        <v>151.6999704693069</v>
       </c>
       <c r="I4">
-        <v>151.7001224507889</v>
+        <v>151.7000981444945</v>
       </c>
       <c r="J4">
-        <v>151.6999125809424</v>
+        <v>151.6997469824527</v>
       </c>
       <c r="K4">
-        <v>151.70027271151</v>
+        <v>151.700202999736</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -592,34 +592,34 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1858368838087445</v>
+        <v>0.1862189255872833</v>
       </c>
       <c r="C5">
-        <v>0.1857612485571072</v>
+        <v>0.1858928912611811</v>
       </c>
       <c r="D5">
-        <v>0.1861352181072565</v>
+        <v>0.1859445013082248</v>
       </c>
       <c r="E5">
-        <v>0.1859818687051331</v>
+        <v>0.1858468200282911</v>
       </c>
       <c r="F5">
-        <v>0.1857552999294743</v>
+        <v>0.1862223951108492</v>
       </c>
       <c r="G5">
-        <v>0.1856863649344985</v>
+        <v>0.1860628828289331</v>
       </c>
       <c r="H5">
-        <v>0.1861521677959577</v>
+        <v>0.1863756125851548</v>
       </c>
       <c r="I5">
-        <v>0.1856683418718548</v>
+        <v>0.1858475716368888</v>
       </c>
       <c r="J5">
-        <v>0.1860409017906546</v>
+        <v>0.1860806893656513</v>
       </c>
       <c r="K5">
-        <v>0.1859057211005391</v>
+        <v>0.1858205056049669</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -627,34 +627,34 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.259973948643365</v>
+        <v>2.259978956548998</v>
       </c>
       <c r="C6">
-        <v>2.26002516094675</v>
+        <v>2.259947803643975</v>
       </c>
       <c r="D6">
-        <v>2.259999111698572</v>
+        <v>2.260025809546947</v>
       </c>
       <c r="E6">
-        <v>2.260000311724449</v>
+        <v>2.259991621672407</v>
       </c>
       <c r="F6">
-        <v>2.259959163109905</v>
+        <v>2.259991958868862</v>
       </c>
       <c r="G6">
-        <v>2.260047096355497</v>
+        <v>2.259995681448602</v>
       </c>
       <c r="H6">
-        <v>2.259988899896379</v>
+        <v>2.260003153490685</v>
       </c>
       <c r="I6">
-        <v>2.259983314538425</v>
+        <v>2.260001686314588</v>
       </c>
       <c r="J6">
-        <v>2.260014812358707</v>
+        <v>2.259988627308207</v>
       </c>
       <c r="K6">
-        <v>2.259992915945571</v>
+        <v>2.259967125538838</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -662,34 +662,34 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3.462238001823559</v>
+        <v>3.455745646189116</v>
       </c>
       <c r="C7">
-        <v>3.452195001774763</v>
+        <v>3.4538418019611</v>
       </c>
       <c r="D7">
-        <v>3.455309570152609</v>
+        <v>3.457080227861884</v>
       </c>
       <c r="E7">
-        <v>3.459601852494266</v>
+        <v>3.447500445080942</v>
       </c>
       <c r="F7">
-        <v>3.450510303292677</v>
+        <v>3.45747422693751</v>
       </c>
       <c r="G7">
-        <v>3.451801201601093</v>
+        <v>3.458169988661405</v>
       </c>
       <c r="H7">
-        <v>3.458783186322658</v>
+        <v>3.467814388736302</v>
       </c>
       <c r="I7">
-        <v>3.464771685033573</v>
+        <v>3.458615841995616</v>
       </c>
       <c r="J7">
-        <v>3.452007808214394</v>
+        <v>3.464834289877412</v>
       </c>
       <c r="K7">
-        <v>3.461366564559452</v>
+        <v>3.448615730143163</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -697,34 +697,34 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>28.35328246627965</v>
+        <v>28.34149517969925</v>
       </c>
       <c r="C8">
-        <v>28.3613210539342</v>
+        <v>28.34600323693632</v>
       </c>
       <c r="D8">
-        <v>28.34979368789626</v>
+        <v>28.34203323028843</v>
       </c>
       <c r="E8">
-        <v>28.35385214930792</v>
+        <v>28.34682029236226</v>
       </c>
       <c r="F8">
-        <v>28.34502265826758</v>
+        <v>28.35125499204733</v>
       </c>
       <c r="G8">
-        <v>28.34550988418791</v>
+        <v>28.3493695122859</v>
       </c>
       <c r="H8">
-        <v>28.35620208116046</v>
+        <v>28.34484277081267</v>
       </c>
       <c r="I8">
-        <v>28.3382920501941</v>
+        <v>28.34437322392657</v>
       </c>
       <c r="J8">
-        <v>28.35422507419655</v>
+        <v>28.34862447957934</v>
       </c>
       <c r="K8">
-        <v>28.34206348646941</v>
+        <v>28.34653999622123</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -732,34 +732,34 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.093177709856165</v>
+        <v>1.054893060672978</v>
       </c>
       <c r="C9">
-        <v>1.001492061027477</v>
+        <v>0.9901695260328268</v>
       </c>
       <c r="D9">
-        <v>1.114531093443119</v>
+        <v>0.9567270305010259</v>
       </c>
       <c r="E9">
-        <v>1.02194587431068</v>
+        <v>0.9470885579604263</v>
       </c>
       <c r="F9">
-        <v>0.9737131157195891</v>
+        <v>0.9933299886754769</v>
       </c>
       <c r="G9">
-        <v>1.060680279480575</v>
+        <v>1.035350823035597</v>
       </c>
       <c r="H9">
-        <v>0.9609457914473327</v>
+        <v>0.9997948843247114</v>
       </c>
       <c r="I9">
-        <v>0.9231960169325319</v>
+        <v>0.9441960484205024</v>
       </c>
       <c r="J9">
-        <v>0.9866590077079703</v>
+        <v>0.9849747474785377</v>
       </c>
       <c r="K9">
-        <v>0.9619534875625357</v>
+        <v>1.087694994123495</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -767,34 +767,34 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.9830189666723926</v>
+        <v>1.020750325171829</v>
       </c>
       <c r="C10">
-        <v>1.000469587177542</v>
+        <v>0.9728458567486176</v>
       </c>
       <c r="D10">
-        <v>1.09670887572522</v>
+        <v>1.003783298085236</v>
       </c>
       <c r="E10">
-        <v>1.040874479637793</v>
+        <v>1.026090065753483</v>
       </c>
       <c r="F10">
-        <v>1.006453283011459</v>
+        <v>1.017438874152209</v>
       </c>
       <c r="G10">
-        <v>1.049750609541351</v>
+        <v>1.046358272401138</v>
       </c>
       <c r="H10">
-        <v>0.9986053634092434</v>
+        <v>0.9164073345367773</v>
       </c>
       <c r="I10">
-        <v>1.023672733825093</v>
+        <v>0.9611634807149179</v>
       </c>
       <c r="J10">
-        <v>1.020503063639943</v>
+        <v>0.9723198136725411</v>
       </c>
       <c r="K10">
-        <v>0.9200515353467695</v>
+        <v>1.037572032976262</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -802,34 +802,34 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2.148137326281182</v>
+        <v>2.147879753816575</v>
       </c>
       <c r="C11">
-        <v>2.148062715985798</v>
+        <v>2.14829058063013</v>
       </c>
       <c r="D11">
-        <v>2.148474998445372</v>
+        <v>2.148080529812282</v>
       </c>
       <c r="E11">
-        <v>2.147721587864839</v>
+        <v>2.147351018910137</v>
       </c>
       <c r="F11">
-        <v>2.147992852194362</v>
+        <v>2.147855378297125</v>
       </c>
       <c r="G11">
-        <v>2.147967415116541</v>
+        <v>2.147987784724509</v>
       </c>
       <c r="H11">
-        <v>2.148205080323858</v>
+        <v>2.147658414761472</v>
       </c>
       <c r="I11">
-        <v>2.147615532861538</v>
+        <v>2.148187721279552</v>
       </c>
       <c r="J11">
-        <v>2.148162369702597</v>
+        <v>2.147999747456856</v>
       </c>
       <c r="K11">
-        <v>2.147943140122769</v>
+        <v>2.14798778326946</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -837,34 +837,34 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.9137635401190134</v>
+        <v>0.9139612738735129</v>
       </c>
       <c r="C12">
-        <v>0.9135898320586733</v>
+        <v>0.9141308141535694</v>
       </c>
       <c r="D12">
-        <v>0.9138888498046496</v>
+        <v>0.9137570331794836</v>
       </c>
       <c r="E12">
-        <v>0.913861442248096</v>
+        <v>0.9142453600793168</v>
       </c>
       <c r="F12">
-        <v>0.9143473610711449</v>
+        <v>0.9138734621969352</v>
       </c>
       <c r="G12">
-        <v>0.9139109815985547</v>
+        <v>0.9139983384681722</v>
       </c>
       <c r="H12">
-        <v>0.9140871953805068</v>
+        <v>0.9142160795722186</v>
       </c>
       <c r="I12">
-        <v>0.9142811630041267</v>
+        <v>0.913514465144264</v>
       </c>
       <c r="J12">
-        <v>0.9140361280252663</v>
+        <v>0.9137610718695441</v>
       </c>
       <c r="K12">
-        <v>0.9141795474798856</v>
+        <v>0.914148953896736</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -872,34 +872,34 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.07899797849761779</v>
+        <v>0.07883753746753003</v>
       </c>
       <c r="C13">
-        <v>0.07850072016923458</v>
+        <v>0.07878346463371405</v>
       </c>
       <c r="D13">
-        <v>0.07848309493729351</v>
+        <v>0.0783994454532482</v>
       </c>
       <c r="E13">
-        <v>0.07809087460331031</v>
+        <v>0.07846966065914462</v>
       </c>
       <c r="F13">
-        <v>0.07883910702345569</v>
+        <v>0.07851219254221967</v>
       </c>
       <c r="G13">
-        <v>0.07804162288012437</v>
+        <v>0.07834215430464123</v>
       </c>
       <c r="H13">
-        <v>0.07819208254240732</v>
+        <v>0.07814859624813368</v>
       </c>
       <c r="I13">
-        <v>0.07832534707477662</v>
+        <v>0.07855355496758679</v>
       </c>
       <c r="J13">
-        <v>0.07837720410554523</v>
+        <v>0.07872894157016369</v>
       </c>
       <c r="K13">
-        <v>0.07860864766240375</v>
+        <v>0.07867052785454667</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -977,34 +977,34 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5539861063525088</v>
+        <v>0.5576565864975382</v>
       </c>
       <c r="C16">
-        <v>0.560136904006802</v>
+        <v>0.5633100609088539</v>
       </c>
       <c r="D16">
-        <v>0.5580062286642269</v>
+        <v>0.5588815115937749</v>
       </c>
       <c r="E16">
-        <v>0.5570433846425586</v>
+        <v>0.5576867962724614</v>
       </c>
       <c r="F16">
-        <v>0.5620217000937219</v>
+        <v>0.560422616376396</v>
       </c>
       <c r="G16">
-        <v>0.560896607178456</v>
+        <v>0.5588559601955254</v>
       </c>
       <c r="H16">
-        <v>0.5574868081472699</v>
+        <v>0.5572212847490884</v>
       </c>
       <c r="I16">
-        <v>0.5607496126479385</v>
+        <v>0.5601890530553552</v>
       </c>
       <c r="J16">
-        <v>0.5626026991603472</v>
+        <v>0.5585722765358336</v>
       </c>
       <c r="K16">
-        <v>0.5591202567727639</v>
+        <v>0.5564687248911931</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1012,34 +1012,34 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.1770084636032254</v>
+        <v>0.1830040952688807</v>
       </c>
       <c r="C17">
-        <v>0.1775331119298715</v>
+        <v>0.1771381558664984</v>
       </c>
       <c r="D17">
-        <v>0.1803824901929285</v>
+        <v>0.1765992904134902</v>
       </c>
       <c r="E17">
-        <v>0.1765559443689853</v>
+        <v>0.1732303950356444</v>
       </c>
       <c r="F17">
-        <v>0.1752344424989548</v>
+        <v>0.1773587591978944</v>
       </c>
       <c r="G17">
-        <v>0.1757131405361943</v>
+        <v>0.1799261370085826</v>
       </c>
       <c r="H17">
-        <v>0.1803892065449929</v>
+        <v>0.1784917558264351</v>
       </c>
       <c r="I17">
-        <v>0.176811318121873</v>
+        <v>0.1786046820764243</v>
       </c>
       <c r="J17">
-        <v>0.1794280377502488</v>
+        <v>0.1774204624625202</v>
       </c>
       <c r="K17">
-        <v>0.1786552643836884</v>
+        <v>0.1800391234001976</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1047,34 +1047,34 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.1261942753325961</v>
+        <v>0.1268943294111833</v>
       </c>
       <c r="C18">
-        <v>0.1273164892242013</v>
+        <v>0.1232629646916496</v>
       </c>
       <c r="D18">
-        <v>0.1316231843651155</v>
+        <v>0.1249704558363358</v>
       </c>
       <c r="E18">
-        <v>0.1267073060792834</v>
+        <v>0.1270583826580347</v>
       </c>
       <c r="F18">
-        <v>0.12772272743954</v>
+        <v>0.1274516940911052</v>
       </c>
       <c r="G18">
-        <v>0.1230910333680566</v>
+        <v>0.1299268904040515</v>
       </c>
       <c r="H18">
-        <v>0.1260409762100131</v>
+        <v>0.1245316678432441</v>
       </c>
       <c r="I18">
-        <v>0.1264393445527374</v>
+        <v>0.1276538861124042</v>
       </c>
       <c r="J18">
-        <v>0.1255006408669416</v>
+        <v>0.1268456107855451</v>
       </c>
       <c r="K18">
-        <v>0.1320828031173832</v>
+        <v>0.1237322334651028</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1082,34 +1082,34 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>5.107928495019868</v>
+        <v>5.109179684782307</v>
       </c>
       <c r="C19">
-        <v>5.105534358665813</v>
+        <v>5.106024282484106</v>
       </c>
       <c r="D19">
-        <v>5.110076427884954</v>
+        <v>5.111998841183548</v>
       </c>
       <c r="E19">
-        <v>5.106745686284809</v>
+        <v>5.108910908645012</v>
       </c>
       <c r="F19">
-        <v>5.108020421166935</v>
+        <v>5.109631830802771</v>
       </c>
       <c r="G19">
-        <v>5.107080150881147</v>
+        <v>5.11193395428767</v>
       </c>
       <c r="H19">
-        <v>5.110157678182184</v>
+        <v>5.111053666298283</v>
       </c>
       <c r="I19">
-        <v>5.108635859509281</v>
+        <v>5.109588203232128</v>
       </c>
       <c r="J19">
-        <v>5.108886040124766</v>
+        <v>5.107810953061803</v>
       </c>
       <c r="K19">
-        <v>5.108922181455591</v>
+        <v>5.10922941857446</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1117,34 +1117,34 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-0.2116320453668024</v>
+        <v>0.1324133553472293</v>
       </c>
       <c r="C20">
-        <v>0.1456869141401416</v>
+        <v>0.1328371572755871</v>
       </c>
       <c r="D20">
-        <v>0.09585758882284506</v>
+        <v>0.05118762380836428</v>
       </c>
       <c r="E20">
-        <v>-0.1299342126396376</v>
+        <v>-0.09633486754725967</v>
       </c>
       <c r="F20">
-        <v>-0.1473722416772844</v>
+        <v>-0.03904123956900606</v>
       </c>
       <c r="G20">
-        <v>0.1060138318371217</v>
+        <v>0.0524745477309605</v>
       </c>
       <c r="H20">
-        <v>-0.1306626672969223</v>
+        <v>-0.0112566915984915</v>
       </c>
       <c r="I20">
-        <v>0.05629860697762571</v>
+        <v>0.2504562101824461</v>
       </c>
       <c r="J20">
-        <v>0.04088534002390976</v>
+        <v>-0.007056925270282208</v>
       </c>
       <c r="K20">
-        <v>-0.04727469295563606</v>
+        <v>0.07969269348340677</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1152,34 +1152,34 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.4714339237595677</v>
+        <v>0.4700157997264651</v>
       </c>
       <c r="C21">
-        <v>0.4666022366363974</v>
+        <v>0.4701253495676302</v>
       </c>
       <c r="D21">
-        <v>0.4657426745662162</v>
+        <v>0.4671535042294674</v>
       </c>
       <c r="E21">
-        <v>0.4705921220262674</v>
+        <v>0.4685985151338783</v>
       </c>
       <c r="F21">
-        <v>0.4652275086401936</v>
+        <v>0.4665790770971511</v>
       </c>
       <c r="G21">
-        <v>0.4663660606929347</v>
+        <v>0.4714427342763881</v>
       </c>
       <c r="H21">
-        <v>0.4670375048529805</v>
+        <v>0.4674770048893905</v>
       </c>
       <c r="I21">
-        <v>0.4656810668672136</v>
+        <v>0.4725311305288477</v>
       </c>
       <c r="J21">
-        <v>0.4663360374332519</v>
+        <v>0.4694740432228472</v>
       </c>
       <c r="K21">
-        <v>0.4712716529556545</v>
+        <v>0.4697261907720746</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1187,34 +1187,34 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>28.34969986740616</v>
+        <v>28.3503960865675</v>
       </c>
       <c r="C22">
-        <v>28.34804303139281</v>
+        <v>28.34974647385031</v>
       </c>
       <c r="D22">
-        <v>28.34608042795394</v>
+        <v>28.34717887525746</v>
       </c>
       <c r="E22">
-        <v>28.34757135893957</v>
+        <v>28.34994216741114</v>
       </c>
       <c r="F22">
-        <v>28.34937965590751</v>
+        <v>28.34775950250226</v>
       </c>
       <c r="G22">
-        <v>28.34701356710595</v>
+        <v>28.35249943762241</v>
       </c>
       <c r="H22">
-        <v>28.35013640518989</v>
+        <v>28.34746248936294</v>
       </c>
       <c r="I22">
-        <v>28.35352651306152</v>
+        <v>28.34938640843791</v>
       </c>
       <c r="J22">
-        <v>28.34973124719988</v>
+        <v>28.34854767964319</v>
       </c>
       <c r="K22">
-        <v>28.34960326290361</v>
+        <v>28.35046137697946</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1222,34 +1222,34 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>29.29992211996989</v>
+        <v>29.29949725238135</v>
       </c>
       <c r="C23">
-        <v>29.29998593122462</v>
+        <v>29.29981193341716</v>
       </c>
       <c r="D23">
-        <v>29.29992355892497</v>
+        <v>29.2993891657513</v>
       </c>
       <c r="E23">
-        <v>29.29992811076993</v>
+        <v>29.29990086160204</v>
       </c>
       <c r="F23">
-        <v>29.29991212757146</v>
+        <v>29.2995960721451</v>
       </c>
       <c r="G23">
-        <v>29.29966092342943</v>
+        <v>29.29982115425189</v>
       </c>
       <c r="H23">
-        <v>29.29952693450764</v>
+        <v>29.29974150688724</v>
       </c>
       <c r="I23">
-        <v>29.29990678828567</v>
+        <v>29.29995811040562</v>
       </c>
       <c r="J23">
-        <v>29.29989835238034</v>
+        <v>29.29974324671636</v>
       </c>
       <c r="K23">
-        <v>29.29944180754087</v>
+        <v>29.299574704669</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1257,34 +1257,34 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.08193734464827018</v>
+        <v>0.08174658975315266</v>
       </c>
       <c r="C24">
-        <v>0.08173362425230453</v>
+        <v>0.08170380220051141</v>
       </c>
       <c r="D24">
-        <v>0.08170919537541398</v>
+        <v>0.08169140504162738</v>
       </c>
       <c r="E24">
-        <v>0.08195381228979351</v>
+        <v>0.08179647306975586</v>
       </c>
       <c r="F24">
-        <v>0.08189228550450754</v>
+        <v>0.0815718403828106</v>
       </c>
       <c r="G24">
-        <v>0.08179881135573124</v>
+        <v>0.08176535651592352</v>
       </c>
       <c r="H24">
-        <v>0.08211748540310322</v>
+        <v>0.08171513684382919</v>
       </c>
       <c r="I24">
-        <v>0.0818274794548932</v>
+        <v>0.08179026338080976</v>
       </c>
       <c r="J24">
-        <v>0.08185916301977177</v>
+        <v>0.08202508220162838</v>
       </c>
       <c r="K24">
-        <v>0.0815719359217746</v>
+        <v>0.08179395886351161</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1292,34 +1292,34 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.4546424153120914</v>
+        <v>0.4547600079597479</v>
       </c>
       <c r="C25">
-        <v>0.4547817962135575</v>
+        <v>0.4544831086340252</v>
       </c>
       <c r="D25">
-        <v>0.4544299103647176</v>
+        <v>0.4546530017005919</v>
       </c>
       <c r="E25">
-        <v>0.4550057597262343</v>
+        <v>0.4545503793727729</v>
       </c>
       <c r="F25">
-        <v>0.4547940930914486</v>
+        <v>0.4549104392728964</v>
       </c>
       <c r="G25">
-        <v>0.4544433113156088</v>
+        <v>0.4549378254922268</v>
       </c>
       <c r="H25">
-        <v>0.4546629487297013</v>
+        <v>0.4547018354555909</v>
       </c>
       <c r="I25">
-        <v>0.4547513333653835</v>
+        <v>0.4546528606764303</v>
       </c>
       <c r="J25">
-        <v>0.4545551292572754</v>
+        <v>0.454801514652259</v>
       </c>
       <c r="K25">
-        <v>0.4544412132004367</v>
+        <v>0.4544479986248605</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1327,34 +1327,34 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1.705594475203555</v>
+        <v>1.707703506651509</v>
       </c>
       <c r="C26">
-        <v>1.70586636027622</v>
+        <v>1.707691745726056</v>
       </c>
       <c r="D26">
-        <v>1.706603564709175</v>
+        <v>1.706117019046336</v>
       </c>
       <c r="E26">
-        <v>1.706714984422249</v>
+        <v>1.707515585143704</v>
       </c>
       <c r="F26">
-        <v>1.707823841228685</v>
+        <v>1.707332040637464</v>
       </c>
       <c r="G26">
-        <v>1.705663136081387</v>
+        <v>1.706727093906057</v>
       </c>
       <c r="H26">
-        <v>1.706372869181645</v>
+        <v>1.706213745649687</v>
       </c>
       <c r="I26">
-        <v>1.706446825596812</v>
+        <v>1.705094302734099</v>
       </c>
       <c r="J26">
-        <v>1.7050831792074</v>
+        <v>1.707396743575549</v>
       </c>
       <c r="K26">
-        <v>1.707140640851524</v>
+        <v>1.707522414691627</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1362,34 +1362,34 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3.592368918162386</v>
+        <v>3.593481302831767</v>
       </c>
       <c r="C27">
-        <v>3.596506307027389</v>
+        <v>3.597590800280476</v>
       </c>
       <c r="D27">
-        <v>3.592489704879585</v>
+        <v>3.598657451636681</v>
       </c>
       <c r="E27">
-        <v>3.594284267150496</v>
+        <v>3.597470665698645</v>
       </c>
       <c r="F27">
-        <v>3.596194681012778</v>
+        <v>3.598732142913191</v>
       </c>
       <c r="G27">
-        <v>3.593598679423529</v>
+        <v>3.59844521142618</v>
       </c>
       <c r="H27">
-        <v>3.594525322887383</v>
+        <v>3.595291464888065</v>
       </c>
       <c r="I27">
-        <v>3.59669062566285</v>
+        <v>3.596205275631936</v>
       </c>
       <c r="J27">
-        <v>3.59606153197772</v>
+        <v>3.596863413265817</v>
       </c>
       <c r="K27">
-        <v>3.596367714154538</v>
+        <v>3.596291359354466</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1397,34 +1397,34 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>12.06653635942964</v>
+        <v>12.06383534319114</v>
       </c>
       <c r="C28">
-        <v>12.06570632240781</v>
+        <v>12.06521140626647</v>
       </c>
       <c r="D28">
-        <v>12.06716251252658</v>
+        <v>12.06587994686345</v>
       </c>
       <c r="E28">
-        <v>12.06686295903804</v>
+        <v>12.0682876407224</v>
       </c>
       <c r="F28">
-        <v>12.06754433494923</v>
+        <v>12.06630324778098</v>
       </c>
       <c r="G28">
-        <v>12.06751331083881</v>
+        <v>12.06660757437342</v>
       </c>
       <c r="H28">
-        <v>12.06500700375633</v>
+        <v>12.06543645307338</v>
       </c>
       <c r="I28">
-        <v>12.06644293497837</v>
+        <v>12.06688977781208</v>
       </c>
       <c r="J28">
-        <v>12.06823499740583</v>
+        <v>12.06720934196149</v>
       </c>
       <c r="K28">
-        <v>12.06564954447934</v>
+        <v>12.06491220049909</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1432,34 +1432,34 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>33.71481999595152</v>
+        <v>34.14603570461778</v>
       </c>
       <c r="C29">
-        <v>34.40179334246634</v>
+        <v>32.26978402882249</v>
       </c>
       <c r="D29">
-        <v>33.73201458080746</v>
+        <v>33.81107365568219</v>
       </c>
       <c r="E29">
-        <v>33.12789810114613</v>
+        <v>33.13077653649592</v>
       </c>
       <c r="F29">
-        <v>33.07977216927241</v>
+        <v>33.22928466163405</v>
       </c>
       <c r="G29">
-        <v>33.54997401483654</v>
+        <v>32.88684030288837</v>
       </c>
       <c r="H29">
-        <v>33.58400560420415</v>
+        <v>33.34493675625605</v>
       </c>
       <c r="I29">
-        <v>33.34797128884055</v>
+        <v>34.05497754656431</v>
       </c>
       <c r="J29">
-        <v>33.07637590469347</v>
+        <v>33.69985762877778</v>
       </c>
       <c r="K29">
-        <v>33.88337302426233</v>
+        <v>33.62311331744729</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1467,34 +1467,34 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>73833.08304917994</v>
+        <v>73829.71093252071</v>
       </c>
       <c r="C30">
-        <v>73868.53096441955</v>
+        <v>73829.63604058954</v>
       </c>
       <c r="D30">
-        <v>73764.63615978623</v>
+        <v>73828.41793003421</v>
       </c>
       <c r="E30">
-        <v>73753.18532026226</v>
+        <v>73830.92313660288</v>
       </c>
       <c r="F30">
-        <v>73866.9601351523</v>
+        <v>73828.7040099259</v>
       </c>
       <c r="G30">
-        <v>73830.14403562009</v>
+        <v>73828.50699865502</v>
       </c>
       <c r="H30">
-        <v>73871.23416343324</v>
+        <v>73830.36091516042</v>
       </c>
       <c r="I30">
-        <v>73785.39942194283</v>
+        <v>73828.17861904409</v>
       </c>
       <c r="J30">
-        <v>73910.16964409599</v>
+        <v>73829.8527951484</v>
       </c>
       <c r="K30">
-        <v>73823.83583773361</v>
+        <v>73826.12022631608</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1502,34 +1502,34 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6.094950182064149</v>
+        <v>6.094284955736032</v>
       </c>
       <c r="C31">
-        <v>6.100176764192717</v>
+        <v>6.096754348103729</v>
       </c>
       <c r="D31">
-        <v>6.095708443434438</v>
+        <v>6.095241783170121</v>
       </c>
       <c r="E31">
-        <v>6.094418489551487</v>
+        <v>6.097225077345534</v>
       </c>
       <c r="F31">
-        <v>6.09358957778096</v>
+        <v>6.094347217377899</v>
       </c>
       <c r="G31">
-        <v>6.097688828145354</v>
+        <v>6.096035433667985</v>
       </c>
       <c r="H31">
-        <v>6.095962020231683</v>
+        <v>6.097752705844488</v>
       </c>
       <c r="I31">
-        <v>6.100963056833723</v>
+        <v>6.097612954487511</v>
       </c>
       <c r="J31">
-        <v>6.09964177845472</v>
+        <v>6.097786880259595</v>
       </c>
       <c r="K31">
-        <v>6.102297150310259</v>
+        <v>6.096403344119373</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1537,34 +1537,34 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>87.79954054668578</v>
+        <v>88.57855820089982</v>
       </c>
       <c r="C32">
-        <v>88.38236884985625</v>
+        <v>88.05621252861096</v>
       </c>
       <c r="D32">
-        <v>87.63967753452461</v>
+        <v>87.93719225694664</v>
       </c>
       <c r="E32">
-        <v>88.10044071904308</v>
+        <v>87.6703527526241</v>
       </c>
       <c r="F32">
-        <v>87.93782724552588</v>
+        <v>88.00296975414125</v>
       </c>
       <c r="G32">
-        <v>88.19931080868989</v>
+        <v>87.73528691898473</v>
       </c>
       <c r="H32">
-        <v>87.32523450711402</v>
+        <v>88.00974678569146</v>
       </c>
       <c r="I32">
-        <v>87.88736185554575</v>
+        <v>87.90290950038045</v>
       </c>
       <c r="J32">
-        <v>87.96355374166792</v>
+        <v>87.96722779893344</v>
       </c>
       <c r="K32">
-        <v>87.83456655828368</v>
+        <v>88.24183443303092</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1572,34 +1572,34 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>50.00041780811303</v>
+        <v>49.99843517431462</v>
       </c>
       <c r="C33">
-        <v>49.99772158526948</v>
+        <v>49.99739473707395</v>
       </c>
       <c r="D33">
-        <v>50.00230365252542</v>
+        <v>49.99802655984951</v>
       </c>
       <c r="E33">
-        <v>50.0017343813136</v>
+        <v>50.00056769089787</v>
       </c>
       <c r="F33">
-        <v>49.99824090219403</v>
+        <v>49.99704119433527</v>
       </c>
       <c r="G33">
-        <v>49.99902702985916</v>
+        <v>49.99913638477914</v>
       </c>
       <c r="H33">
-        <v>50.00017648139909</v>
+        <v>50.00168968657443</v>
       </c>
       <c r="I33">
-        <v>49.99745453179378</v>
+        <v>49.99960672183818</v>
       </c>
       <c r="J33">
-        <v>50.00109479256857</v>
+        <v>50.00734347802332</v>
       </c>
       <c r="K33">
-        <v>50.00184872984421</v>
+        <v>50.00066299428491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   Outputs/MonteCarlo_sim_inputs.xlsx 	modified:   Outputs/MonteCarlo_sim_outputs.xlsx
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_inputs.xlsx
+++ b/Outputs/MonteCarlo_sim_inputs.xlsx
@@ -487,34 +487,34 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.07817971878511421</v>
+        <v>0.07829464001795738</v>
       </c>
       <c r="C2">
-        <v>0.0783311784570309</v>
+        <v>0.07877937800938027</v>
       </c>
       <c r="D2">
-        <v>0.07882964468300416</v>
+        <v>0.07864014179500259</v>
       </c>
       <c r="E2">
-        <v>0.07898575576335547</v>
+        <v>0.07845946774641657</v>
       </c>
       <c r="F2">
-        <v>0.0789021773171731</v>
+        <v>0.07839212744846909</v>
       </c>
       <c r="G2">
-        <v>0.07841102167452746</v>
+        <v>0.07822152187813221</v>
       </c>
       <c r="H2">
-        <v>0.07816076904529083</v>
+        <v>0.07854383010459076</v>
       </c>
       <c r="I2">
-        <v>0.07902881765877712</v>
+        <v>0.07873393418916634</v>
       </c>
       <c r="J2">
-        <v>0.07869720463851246</v>
+        <v>0.07847923265723404</v>
       </c>
       <c r="K2">
-        <v>0.07807812593315568</v>
+        <v>0.0789098965158269</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -522,34 +522,34 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>25.8498244400453</v>
+        <v>25.85019593345956</v>
       </c>
       <c r="C3">
-        <v>25.84895386915952</v>
+        <v>25.85070029556539</v>
       </c>
       <c r="D3">
-        <v>25.85227483928836</v>
+        <v>25.85099975479828</v>
       </c>
       <c r="E3">
-        <v>25.84965830012807</v>
+        <v>25.84861473840749</v>
       </c>
       <c r="F3">
-        <v>25.84939258695979</v>
+        <v>25.84971866607145</v>
       </c>
       <c r="G3">
-        <v>25.84872764592898</v>
+        <v>25.85125078759752</v>
       </c>
       <c r="H3">
-        <v>25.84893176529916</v>
+        <v>25.85014495677666</v>
       </c>
       <c r="I3">
-        <v>25.84849984402901</v>
+        <v>25.84863092719272</v>
       </c>
       <c r="J3">
-        <v>25.84851247639706</v>
+        <v>25.85136409568195</v>
       </c>
       <c r="K3">
-        <v>25.84989010061628</v>
+        <v>25.8508551500793</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -557,34 +557,34 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>151.6999409060293</v>
+        <v>151.6999346847188</v>
       </c>
       <c r="C4">
-        <v>151.6996680895456</v>
+        <v>151.7000764647251</v>
       </c>
       <c r="D4">
-        <v>151.7001258504768</v>
+        <v>151.7002375642224</v>
       </c>
       <c r="E4">
-        <v>151.7002862504015</v>
+        <v>151.7001719018875</v>
       </c>
       <c r="F4">
-        <v>151.6999693512639</v>
+        <v>151.7003755474327</v>
       </c>
       <c r="G4">
-        <v>151.6999072420455</v>
+        <v>151.7003002664522</v>
       </c>
       <c r="H4">
-        <v>151.6999704693069</v>
+        <v>151.6996346577992</v>
       </c>
       <c r="I4">
-        <v>151.7000981444945</v>
+        <v>151.700029767051</v>
       </c>
       <c r="J4">
-        <v>151.6997469824527</v>
+        <v>151.7001880554535</v>
       </c>
       <c r="K4">
-        <v>151.700202999736</v>
+        <v>151.6998287745109</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -592,34 +592,34 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1862189255872833</v>
+        <v>0.1860831622481827</v>
       </c>
       <c r="C5">
-        <v>0.1858928912611811</v>
+        <v>0.1862753780545544</v>
       </c>
       <c r="D5">
-        <v>0.1859445013082248</v>
+        <v>0.1857153692294063</v>
       </c>
       <c r="E5">
-        <v>0.1858468200282911</v>
+        <v>0.1858021064205384</v>
       </c>
       <c r="F5">
-        <v>0.1862223951108492</v>
+        <v>0.1859662790003875</v>
       </c>
       <c r="G5">
-        <v>0.1860628828289331</v>
+        <v>0.1858419944894474</v>
       </c>
       <c r="H5">
-        <v>0.1863756125851548</v>
+        <v>0.1862059983888287</v>
       </c>
       <c r="I5">
-        <v>0.1858475716368888</v>
+        <v>0.185682111945499</v>
       </c>
       <c r="J5">
-        <v>0.1860806893656513</v>
+        <v>0.185744846220143</v>
       </c>
       <c r="K5">
-        <v>0.1858205056049669</v>
+        <v>0.1862053133238964</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -627,34 +627,34 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.259978956548998</v>
+        <v>2.26001763044322</v>
       </c>
       <c r="C6">
-        <v>2.259947803643975</v>
+        <v>2.260004186377163</v>
       </c>
       <c r="D6">
-        <v>2.260025809546947</v>
+        <v>2.260054718534799</v>
       </c>
       <c r="E6">
-        <v>2.259991621672407</v>
+        <v>2.260063664649345</v>
       </c>
       <c r="F6">
-        <v>2.259991958868862</v>
+        <v>2.25999867772061</v>
       </c>
       <c r="G6">
-        <v>2.259995681448602</v>
+        <v>2.259959387229524</v>
       </c>
       <c r="H6">
-        <v>2.260003153490685</v>
+        <v>2.259987328146046</v>
       </c>
       <c r="I6">
-        <v>2.260001686314588</v>
+        <v>2.260002012944936</v>
       </c>
       <c r="J6">
-        <v>2.259988627308207</v>
+        <v>2.260034208203687</v>
       </c>
       <c r="K6">
-        <v>2.259967125538838</v>
+        <v>2.260024586863321</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -662,34 +662,34 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3.455745646189116</v>
+        <v>3.453675847372491</v>
       </c>
       <c r="C7">
-        <v>3.4538418019611</v>
+        <v>3.455541528031846</v>
       </c>
       <c r="D7">
-        <v>3.457080227861884</v>
+        <v>3.457999755294844</v>
       </c>
       <c r="E7">
-        <v>3.447500445080942</v>
+        <v>3.456235084187883</v>
       </c>
       <c r="F7">
-        <v>3.45747422693751</v>
+        <v>3.452212508390573</v>
       </c>
       <c r="G7">
-        <v>3.458169988661405</v>
+        <v>3.457980330006651</v>
       </c>
       <c r="H7">
-        <v>3.467814388736302</v>
+        <v>3.451763697386524</v>
       </c>
       <c r="I7">
-        <v>3.458615841995616</v>
+        <v>3.464101212240302</v>
       </c>
       <c r="J7">
-        <v>3.464834289877412</v>
+        <v>3.452743040987104</v>
       </c>
       <c r="K7">
-        <v>3.448615730143163</v>
+        <v>3.447870103102793</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -697,34 +697,34 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>28.34149517969925</v>
+        <v>28.34962624529889</v>
       </c>
       <c r="C8">
-        <v>28.34600323693632</v>
+        <v>28.344000833388</v>
       </c>
       <c r="D8">
-        <v>28.34203323028843</v>
+        <v>28.34835403664405</v>
       </c>
       <c r="E8">
-        <v>28.34682029236226</v>
+        <v>28.35635819023252</v>
       </c>
       <c r="F8">
-        <v>28.35125499204733</v>
+        <v>28.3519181595647</v>
       </c>
       <c r="G8">
-        <v>28.3493695122859</v>
+        <v>28.34910650015055</v>
       </c>
       <c r="H8">
-        <v>28.34484277081267</v>
+        <v>28.34433914755335</v>
       </c>
       <c r="I8">
-        <v>28.34437322392657</v>
+        <v>28.35180112008402</v>
       </c>
       <c r="J8">
-        <v>28.34862447957934</v>
+        <v>28.35099152884476</v>
       </c>
       <c r="K8">
-        <v>28.34653999622123</v>
+        <v>28.35002394003423</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -732,34 +732,34 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.054893060672978</v>
+        <v>1.019583450301445</v>
       </c>
       <c r="C9">
-        <v>0.9901695260328268</v>
+        <v>0.9822501316885365</v>
       </c>
       <c r="D9">
-        <v>0.9567270305010259</v>
+        <v>0.9261442989850726</v>
       </c>
       <c r="E9">
-        <v>0.9470885579604263</v>
+        <v>1.047552846343779</v>
       </c>
       <c r="F9">
-        <v>0.9933299886754769</v>
+        <v>0.9520601549159953</v>
       </c>
       <c r="G9">
-        <v>1.035350823035597</v>
+        <v>1.006742665056656</v>
       </c>
       <c r="H9">
-        <v>0.9997948843247114</v>
+        <v>1.044927020788788</v>
       </c>
       <c r="I9">
-        <v>0.9441960484205024</v>
+        <v>0.9707211411912515</v>
       </c>
       <c r="J9">
-        <v>0.9849747474785377</v>
+        <v>0.9545144623237745</v>
       </c>
       <c r="K9">
-        <v>1.087694994123495</v>
+        <v>1.084428070334901</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -767,34 +767,34 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.020750325171829</v>
+        <v>1.007534181037856</v>
       </c>
       <c r="C10">
-        <v>0.9728458567486176</v>
+        <v>0.9546461279385999</v>
       </c>
       <c r="D10">
-        <v>1.003783298085236</v>
+        <v>0.9719281590415387</v>
       </c>
       <c r="E10">
-        <v>1.026090065753483</v>
+        <v>0.9721441075529493</v>
       </c>
       <c r="F10">
-        <v>1.017438874152209</v>
+        <v>1.046107470645524</v>
       </c>
       <c r="G10">
-        <v>1.046358272401138</v>
+        <v>1.034610389099874</v>
       </c>
       <c r="H10">
-        <v>0.9164073345367773</v>
+        <v>0.9371348491067988</v>
       </c>
       <c r="I10">
-        <v>0.9611634807149179</v>
+        <v>0.9632213719002793</v>
       </c>
       <c r="J10">
-        <v>0.9723198136725411</v>
+        <v>1.072636439813636</v>
       </c>
       <c r="K10">
-        <v>1.037572032976262</v>
+        <v>0.9336179197863443</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -802,34 +802,34 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2.147879753816575</v>
+        <v>2.148271484035093</v>
       </c>
       <c r="C11">
-        <v>2.14829058063013</v>
+        <v>2.147482920061125</v>
       </c>
       <c r="D11">
-        <v>2.148080529812282</v>
+        <v>2.148346146262153</v>
       </c>
       <c r="E11">
-        <v>2.147351018910137</v>
+        <v>2.147891282509959</v>
       </c>
       <c r="F11">
-        <v>2.147855378297125</v>
+        <v>2.148129718447739</v>
       </c>
       <c r="G11">
-        <v>2.147987784724509</v>
+        <v>2.148097846148703</v>
       </c>
       <c r="H11">
-        <v>2.147658414761472</v>
+        <v>2.147756030947023</v>
       </c>
       <c r="I11">
-        <v>2.148187721279552</v>
+        <v>2.148159141364875</v>
       </c>
       <c r="J11">
-        <v>2.147999747456856</v>
+        <v>2.147436942348215</v>
       </c>
       <c r="K11">
-        <v>2.14798778326946</v>
+        <v>2.147558505758274</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -837,34 +837,34 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.9139612738735129</v>
+        <v>0.9139772165975671</v>
       </c>
       <c r="C12">
-        <v>0.9141308141535694</v>
+        <v>0.9141457440875383</v>
       </c>
       <c r="D12">
-        <v>0.9137570331794836</v>
+        <v>0.9138312621800739</v>
       </c>
       <c r="E12">
-        <v>0.9142453600793168</v>
+        <v>0.9139871782117261</v>
       </c>
       <c r="F12">
-        <v>0.9138734621969352</v>
+        <v>0.914051946331627</v>
       </c>
       <c r="G12">
-        <v>0.9139983384681722</v>
+        <v>0.914302973228477</v>
       </c>
       <c r="H12">
-        <v>0.9142160795722186</v>
+        <v>0.9140506423466492</v>
       </c>
       <c r="I12">
-        <v>0.913514465144264</v>
+        <v>0.9142077091995608</v>
       </c>
       <c r="J12">
-        <v>0.9137610718695441</v>
+        <v>0.9138909900399609</v>
       </c>
       <c r="K12">
-        <v>0.914148953896736</v>
+        <v>0.9143307422070915</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -872,34 +872,34 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.07883753746753003</v>
+        <v>0.07853833481992255</v>
       </c>
       <c r="C13">
-        <v>0.07878346463371405</v>
+        <v>0.07861817272536452</v>
       </c>
       <c r="D13">
-        <v>0.0783994454532482</v>
+        <v>0.07841600278424737</v>
       </c>
       <c r="E13">
-        <v>0.07846966065914462</v>
+        <v>0.07777917458271301</v>
       </c>
       <c r="F13">
-        <v>0.07851219254221967</v>
+        <v>0.07871781409027048</v>
       </c>
       <c r="G13">
-        <v>0.07834215430464123</v>
+        <v>0.07868380093850569</v>
       </c>
       <c r="H13">
-        <v>0.07814859624813368</v>
+        <v>0.07878864845778275</v>
       </c>
       <c r="I13">
-        <v>0.07855355496758679</v>
+        <v>0.07886209056618407</v>
       </c>
       <c r="J13">
-        <v>0.07872894157016369</v>
+        <v>0.07879170469206687</v>
       </c>
       <c r="K13">
-        <v>0.07867052785454667</v>
+        <v>0.07831237626461238</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -977,34 +977,34 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5576565864975382</v>
+        <v>0.5573914293617266</v>
       </c>
       <c r="C16">
-        <v>0.5633100609088539</v>
+        <v>0.5574819437438194</v>
       </c>
       <c r="D16">
-        <v>0.5588815115937749</v>
+        <v>0.5559152672228114</v>
       </c>
       <c r="E16">
-        <v>0.5576867962724614</v>
+        <v>0.5578127642838832</v>
       </c>
       <c r="F16">
-        <v>0.560422616376396</v>
+        <v>0.557194318724387</v>
       </c>
       <c r="G16">
-        <v>0.5588559601955254</v>
+        <v>0.5560378759442558</v>
       </c>
       <c r="H16">
-        <v>0.5572212847490884</v>
+        <v>0.5574108306746501</v>
       </c>
       <c r="I16">
-        <v>0.5601890530553552</v>
+        <v>0.5600151223014637</v>
       </c>
       <c r="J16">
-        <v>0.5585722765358336</v>
+        <v>0.5593414678296798</v>
       </c>
       <c r="K16">
-        <v>0.5564687248911931</v>
+        <v>0.5547791093697644</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1012,34 +1012,34 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.1830040952688807</v>
+        <v>0.1765566216305918</v>
       </c>
       <c r="C17">
-        <v>0.1771381558664984</v>
+        <v>0.1790828072834728</v>
       </c>
       <c r="D17">
-        <v>0.1765992904134902</v>
+        <v>0.1768632443268893</v>
       </c>
       <c r="E17">
-        <v>0.1732303950356444</v>
+        <v>0.1755092347525782</v>
       </c>
       <c r="F17">
-        <v>0.1773587591978944</v>
+        <v>0.1813022432812508</v>
       </c>
       <c r="G17">
-        <v>0.1799261370085826</v>
+        <v>0.1755682698221086</v>
       </c>
       <c r="H17">
-        <v>0.1784917558264351</v>
+        <v>0.1786419316875567</v>
       </c>
       <c r="I17">
-        <v>0.1786046820764243</v>
+        <v>0.1787515149482427</v>
       </c>
       <c r="J17">
-        <v>0.1774204624625202</v>
+        <v>0.1793819466262752</v>
       </c>
       <c r="K17">
-        <v>0.1800391234001976</v>
+        <v>0.1781278540065145</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1047,34 +1047,34 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.1268943294111833</v>
+        <v>0.1287221680001877</v>
       </c>
       <c r="C18">
-        <v>0.1232629646916496</v>
+        <v>0.1255264507806259</v>
       </c>
       <c r="D18">
-        <v>0.1249704558363358</v>
+        <v>0.1259292100341978</v>
       </c>
       <c r="E18">
-        <v>0.1270583826580347</v>
+        <v>0.1251207486136789</v>
       </c>
       <c r="F18">
-        <v>0.1274516940911052</v>
+        <v>0.1292148721073986</v>
       </c>
       <c r="G18">
-        <v>0.1299268904040515</v>
+        <v>0.1267313761644601</v>
       </c>
       <c r="H18">
-        <v>0.1245316678432441</v>
+        <v>0.1243981675619309</v>
       </c>
       <c r="I18">
-        <v>0.1276538861124042</v>
+        <v>0.1311479043933923</v>
       </c>
       <c r="J18">
-        <v>0.1268456107855451</v>
+        <v>0.125248699610824</v>
       </c>
       <c r="K18">
-        <v>0.1237322334651028</v>
+        <v>0.1283314698565677</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1082,34 +1082,34 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>5.109179684782307</v>
+        <v>5.105778973152722</v>
       </c>
       <c r="C19">
-        <v>5.106024282484106</v>
+        <v>5.109442297168108</v>
       </c>
       <c r="D19">
-        <v>5.111998841183548</v>
+        <v>5.108964955443522</v>
       </c>
       <c r="E19">
-        <v>5.108910908645012</v>
+        <v>5.107837790213064</v>
       </c>
       <c r="F19">
-        <v>5.109631830802771</v>
+        <v>5.113076611127469</v>
       </c>
       <c r="G19">
-        <v>5.11193395428767</v>
+        <v>5.107342658957783</v>
       </c>
       <c r="H19">
-        <v>5.111053666298283</v>
+        <v>5.106851266750354</v>
       </c>
       <c r="I19">
-        <v>5.109588203232128</v>
+        <v>5.108736476894448</v>
       </c>
       <c r="J19">
-        <v>5.107810953061803</v>
+        <v>5.110864059677319</v>
       </c>
       <c r="K19">
-        <v>5.10922941857446</v>
+        <v>5.106624826647602</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1117,34 +1117,34 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.1324133553472293</v>
+        <v>0.03498530696886858</v>
       </c>
       <c r="C20">
-        <v>0.1328371572755871</v>
+        <v>0.04610574957989958</v>
       </c>
       <c r="D20">
-        <v>0.05118762380836428</v>
+        <v>0.01811912589879062</v>
       </c>
       <c r="E20">
-        <v>-0.09633486754725967</v>
+        <v>0.19490294959918</v>
       </c>
       <c r="F20">
-        <v>-0.03904123956900606</v>
+        <v>0.0119782390300526</v>
       </c>
       <c r="G20">
-        <v>0.0524745477309605</v>
+        <v>-0.1735601647493568</v>
       </c>
       <c r="H20">
-        <v>-0.0112566915984915</v>
+        <v>0.1159149686986259</v>
       </c>
       <c r="I20">
-        <v>0.2504562101824461</v>
+        <v>0.008905986893584577</v>
       </c>
       <c r="J20">
-        <v>-0.007056925270282208</v>
+        <v>-0.02052641133729731</v>
       </c>
       <c r="K20">
-        <v>0.07969269348340677</v>
+        <v>-0.1335436431116351</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1152,34 +1152,34 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.4700157997264651</v>
+        <v>0.4717701502357043</v>
       </c>
       <c r="C21">
-        <v>0.4701253495676302</v>
+        <v>0.4673506793146259</v>
       </c>
       <c r="D21">
-        <v>0.4671535042294674</v>
+        <v>0.4696720409254531</v>
       </c>
       <c r="E21">
-        <v>0.4685985151338783</v>
+        <v>0.4677877521550363</v>
       </c>
       <c r="F21">
-        <v>0.4665790770971511</v>
+        <v>0.4690655900286287</v>
       </c>
       <c r="G21">
-        <v>0.4714427342763881</v>
+        <v>0.4688643044983773</v>
       </c>
       <c r="H21">
-        <v>0.4674770048893905</v>
+        <v>0.4676974214842532</v>
       </c>
       <c r="I21">
-        <v>0.4725311305288477</v>
+        <v>0.4704527467522187</v>
       </c>
       <c r="J21">
-        <v>0.4694740432228472</v>
+        <v>0.4662722521868444</v>
       </c>
       <c r="K21">
-        <v>0.4697261907720746</v>
+        <v>0.4676686963059437</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1187,34 +1187,34 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>28.3503960865675</v>
+        <v>28.34777339226817</v>
       </c>
       <c r="C22">
-        <v>28.34974647385031</v>
+        <v>28.35274637830266</v>
       </c>
       <c r="D22">
-        <v>28.34717887525746</v>
+        <v>28.35219107947395</v>
       </c>
       <c r="E22">
-        <v>28.34994216741114</v>
+        <v>28.35472398239264</v>
       </c>
       <c r="F22">
-        <v>28.34775950250226</v>
+        <v>28.34942630968719</v>
       </c>
       <c r="G22">
-        <v>28.35249943762241</v>
+        <v>28.35337801944043</v>
       </c>
       <c r="H22">
-        <v>28.34746248936294</v>
+        <v>28.34793007244464</v>
       </c>
       <c r="I22">
-        <v>28.34938640843791</v>
+        <v>28.35152330430449</v>
       </c>
       <c r="J22">
-        <v>28.34854767964319</v>
+        <v>28.34854285970777</v>
       </c>
       <c r="K22">
-        <v>28.35046137697946</v>
+        <v>28.35073385585933</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1222,34 +1222,34 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>29.29949725238135</v>
+        <v>29.29981278272576</v>
       </c>
       <c r="C23">
-        <v>29.29981193341716</v>
+        <v>29.30003614354623</v>
       </c>
       <c r="D23">
-        <v>29.2993891657513</v>
+        <v>29.29969333681713</v>
       </c>
       <c r="E23">
-        <v>29.29990086160204</v>
+        <v>29.29936336139002</v>
       </c>
       <c r="F23">
-        <v>29.2995960721451</v>
+        <v>29.29979820362986</v>
       </c>
       <c r="G23">
-        <v>29.29982115425189</v>
+        <v>29.29973687814825</v>
       </c>
       <c r="H23">
-        <v>29.29974150688724</v>
+        <v>29.29955298175352</v>
       </c>
       <c r="I23">
-        <v>29.29995811040562</v>
+        <v>29.30012856157847</v>
       </c>
       <c r="J23">
-        <v>29.29974324671636</v>
+        <v>29.30003950881936</v>
       </c>
       <c r="K23">
-        <v>29.299574704669</v>
+        <v>29.30002670310249</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1257,34 +1257,34 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.08174658975315266</v>
+        <v>0.08224020047053716</v>
       </c>
       <c r="C24">
-        <v>0.08170380220051141</v>
+        <v>0.08194636649499315</v>
       </c>
       <c r="D24">
-        <v>0.08169140504162738</v>
+        <v>0.08186422590092685</v>
       </c>
       <c r="E24">
-        <v>0.08179647306975586</v>
+        <v>0.08164065438815642</v>
       </c>
       <c r="F24">
-        <v>0.0815718403828106</v>
+        <v>0.0818511814526624</v>
       </c>
       <c r="G24">
-        <v>0.08176535651592352</v>
+        <v>0.08179044892640952</v>
       </c>
       <c r="H24">
-        <v>0.08171513684382919</v>
+        <v>0.08182374031526424</v>
       </c>
       <c r="I24">
-        <v>0.08179026338080976</v>
+        <v>0.08154988090471246</v>
       </c>
       <c r="J24">
-        <v>0.08202508220162838</v>
+        <v>0.08155819761380108</v>
       </c>
       <c r="K24">
-        <v>0.08179395886351161</v>
+        <v>0.08180848758817866</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1292,34 +1292,34 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.4547600079597479</v>
+        <v>0.454874150029585</v>
       </c>
       <c r="C25">
-        <v>0.4544831086340252</v>
+        <v>0.4545835476838459</v>
       </c>
       <c r="D25">
-        <v>0.4546530017005919</v>
+        <v>0.4546264619438994</v>
       </c>
       <c r="E25">
-        <v>0.4545503793727729</v>
+        <v>0.4545633222288285</v>
       </c>
       <c r="F25">
-        <v>0.4549104392728964</v>
+        <v>0.4547887067399076</v>
       </c>
       <c r="G25">
-        <v>0.4549378254922268</v>
+        <v>0.4549442585330364</v>
       </c>
       <c r="H25">
-        <v>0.4547018354555909</v>
+        <v>0.4546211175806204</v>
       </c>
       <c r="I25">
-        <v>0.4546528606764303</v>
+        <v>0.4547563877505353</v>
       </c>
       <c r="J25">
-        <v>0.454801514652259</v>
+        <v>0.4544312934530398</v>
       </c>
       <c r="K25">
-        <v>0.4544479986248605</v>
+        <v>0.4549797119701208</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1327,34 +1327,34 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1.707703506651509</v>
+        <v>1.705118640554433</v>
       </c>
       <c r="C26">
-        <v>1.707691745726056</v>
+        <v>1.705723267727757</v>
       </c>
       <c r="D26">
-        <v>1.706117019046336</v>
+        <v>1.707485448234782</v>
       </c>
       <c r="E26">
-        <v>1.707515585143704</v>
+        <v>1.705621248318673</v>
       </c>
       <c r="F26">
-        <v>1.707332040637464</v>
+        <v>1.70682642231767</v>
       </c>
       <c r="G26">
-        <v>1.706727093906057</v>
+        <v>1.705593589127088</v>
       </c>
       <c r="H26">
-        <v>1.706213745649687</v>
+        <v>1.706185120607468</v>
       </c>
       <c r="I26">
-        <v>1.705094302734099</v>
+        <v>1.706366849841732</v>
       </c>
       <c r="J26">
-        <v>1.707396743575549</v>
+        <v>1.70677684862712</v>
       </c>
       <c r="K26">
-        <v>1.707522414691627</v>
+        <v>1.706176330402858</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1362,34 +1362,34 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3.593481302831767</v>
+        <v>3.597729040931274</v>
       </c>
       <c r="C27">
-        <v>3.597590800280476</v>
+        <v>3.597175614431924</v>
       </c>
       <c r="D27">
-        <v>3.598657451636681</v>
+        <v>3.593129072449697</v>
       </c>
       <c r="E27">
-        <v>3.597470665698645</v>
+        <v>3.595088140299688</v>
       </c>
       <c r="F27">
-        <v>3.598732142913191</v>
+        <v>3.598501945693067</v>
       </c>
       <c r="G27">
-        <v>3.59844521142618</v>
+        <v>3.597435947351289</v>
       </c>
       <c r="H27">
-        <v>3.595291464888065</v>
+        <v>3.596697499929983</v>
       </c>
       <c r="I27">
-        <v>3.596205275631936</v>
+        <v>3.5909230147504</v>
       </c>
       <c r="J27">
-        <v>3.596863413265817</v>
+        <v>3.598891063330766</v>
       </c>
       <c r="K27">
-        <v>3.596291359354466</v>
+        <v>3.596479512886261</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1397,34 +1397,34 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>12.06383534319114</v>
+        <v>12.066180680864</v>
       </c>
       <c r="C28">
-        <v>12.06521140626647</v>
+        <v>12.06544430953787</v>
       </c>
       <c r="D28">
-        <v>12.06587994686345</v>
+        <v>12.06510201034599</v>
       </c>
       <c r="E28">
-        <v>12.0682876407224</v>
+        <v>12.06534929841172</v>
       </c>
       <c r="F28">
-        <v>12.06630324778098</v>
+        <v>12.06598123951287</v>
       </c>
       <c r="G28">
-        <v>12.06660757437342</v>
+        <v>12.06605208944585</v>
       </c>
       <c r="H28">
-        <v>12.06543645307338</v>
+        <v>12.06489323244117</v>
       </c>
       <c r="I28">
-        <v>12.06688977781208</v>
+        <v>12.06586595339339</v>
       </c>
       <c r="J28">
-        <v>12.06720934196149</v>
+        <v>12.06681303230606</v>
       </c>
       <c r="K28">
-        <v>12.06491220049909</v>
+        <v>12.06605055274717</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1432,34 +1432,34 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>34.14603570461778</v>
+        <v>33.86776796434634</v>
       </c>
       <c r="C29">
-        <v>32.26978402882249</v>
+        <v>34.1073979171316</v>
       </c>
       <c r="D29">
-        <v>33.81107365568219</v>
+        <v>33.47609118997086</v>
       </c>
       <c r="E29">
-        <v>33.13077653649592</v>
+        <v>33.58289528355159</v>
       </c>
       <c r="F29">
-        <v>33.22928466163405</v>
+        <v>33.21084359972032</v>
       </c>
       <c r="G29">
-        <v>32.88684030288837</v>
+        <v>34.2432549357861</v>
       </c>
       <c r="H29">
-        <v>33.34493675625605</v>
+        <v>34.08796274080287</v>
       </c>
       <c r="I29">
-        <v>34.05497754656431</v>
+        <v>33.45285365052489</v>
       </c>
       <c r="J29">
-        <v>33.69985762877778</v>
+        <v>33.24261212657254</v>
       </c>
       <c r="K29">
-        <v>33.62311331744729</v>
+        <v>33.36581112764438</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1467,34 +1467,34 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>73829.71093252071</v>
+        <v>73826.62712876595</v>
       </c>
       <c r="C30">
-        <v>73829.63604058954</v>
+        <v>73830.8632851734</v>
       </c>
       <c r="D30">
-        <v>73828.41793003421</v>
+        <v>73828.07639414954</v>
       </c>
       <c r="E30">
-        <v>73830.92313660288</v>
+        <v>73830.74848240045</v>
       </c>
       <c r="F30">
-        <v>73828.7040099259</v>
+        <v>73827.17590826476</v>
       </c>
       <c r="G30">
-        <v>73828.50699865502</v>
+        <v>73829.79154578631</v>
       </c>
       <c r="H30">
-        <v>73830.36091516042</v>
+        <v>73830.12926429899</v>
       </c>
       <c r="I30">
-        <v>73828.17861904409</v>
+        <v>73826.53576813792</v>
       </c>
       <c r="J30">
-        <v>73829.8527951484</v>
+        <v>73828.99813538382</v>
       </c>
       <c r="K30">
-        <v>73826.12022631608</v>
+        <v>73830.99813201187</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1502,34 +1502,34 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6.094284955736032</v>
+        <v>6.090583347802331</v>
       </c>
       <c r="C31">
-        <v>6.096754348103729</v>
+        <v>6.096809103034817</v>
       </c>
       <c r="D31">
-        <v>6.095241783170121</v>
+        <v>6.094375516301245</v>
       </c>
       <c r="E31">
-        <v>6.097225077345534</v>
+        <v>6.09504423246972</v>
       </c>
       <c r="F31">
-        <v>6.094347217377899</v>
+        <v>6.092399715646361</v>
       </c>
       <c r="G31">
-        <v>6.096035433667985</v>
+        <v>6.092528228495246</v>
       </c>
       <c r="H31">
-        <v>6.097752705844488</v>
+        <v>6.094957554487915</v>
       </c>
       <c r="I31">
-        <v>6.097612954487511</v>
+        <v>6.095546975854501</v>
       </c>
       <c r="J31">
-        <v>6.097786880259595</v>
+        <v>6.098578235393386</v>
       </c>
       <c r="K31">
-        <v>6.096403344119373</v>
+        <v>6.097861709576327</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1537,34 +1537,34 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>88.57855820089982</v>
+        <v>87.66473788957597</v>
       </c>
       <c r="C32">
-        <v>88.05621252861096</v>
+        <v>88.10452110964768</v>
       </c>
       <c r="D32">
-        <v>87.93719225694664</v>
+        <v>87.69285093873057</v>
       </c>
       <c r="E32">
-        <v>87.6703527526241</v>
+        <v>88.13813779289703</v>
       </c>
       <c r="F32">
-        <v>88.00296975414125</v>
+        <v>88.29599320998808</v>
       </c>
       <c r="G32">
-        <v>87.73528691898473</v>
+        <v>88.37249115381557</v>
       </c>
       <c r="H32">
-        <v>88.00974678569146</v>
+        <v>87.79372876961028</v>
       </c>
       <c r="I32">
-        <v>87.90290950038045</v>
+        <v>87.9820387070034</v>
       </c>
       <c r="J32">
-        <v>87.96722779893344</v>
+        <v>88.25966293931403</v>
       </c>
       <c r="K32">
-        <v>88.24183443303092</v>
+        <v>88.18128768123452</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1572,34 +1572,34 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>49.99843517431462</v>
+        <v>50.00164019261909</v>
       </c>
       <c r="C33">
-        <v>49.99739473707395</v>
+        <v>49.99850087994426</v>
       </c>
       <c r="D33">
-        <v>49.99802655984951</v>
+        <v>49.99925892340833</v>
       </c>
       <c r="E33">
-        <v>50.00056769089787</v>
+        <v>49.9996273942193</v>
       </c>
       <c r="F33">
-        <v>49.99704119433527</v>
+        <v>50.0037324980015</v>
       </c>
       <c r="G33">
-        <v>49.99913638477914</v>
+        <v>50.00149993752392</v>
       </c>
       <c r="H33">
-        <v>50.00168968657443</v>
+        <v>49.9990622328394</v>
       </c>
       <c r="I33">
-        <v>49.99960672183818</v>
+        <v>49.99963059861378</v>
       </c>
       <c r="J33">
-        <v>50.00734347802332</v>
+        <v>49.99714851794409</v>
       </c>
       <c r="K33">
-        <v>50.00066299428491</v>
+        <v>49.99862495360775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   MonteCarlo_Sim.py 	modified:   Outputs/MonteCarlo_sim_inputs.xlsx 	modified:   Outputs/MonteCarlo_sim_outputs.xlsx 	modified:   Tools.py
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_inputs.xlsx
+++ b/Outputs/MonteCarlo_sim_inputs.xlsx
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.07842998577292572</v>
+        <v>0.0782454872199231</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -477,7 +477,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>23.13870511119994</v>
+        <v>23.13929419043147</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -485,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>151.7000723364447</v>
+        <v>151.7000066755207</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -493,7 +493,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1858186392533446</v>
+        <v>0.1862698743118686</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -501,7 +501,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.549999075347138</v>
+        <v>2.550013287552345</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -509,7 +509,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.7658985327361176</v>
+        <v>0.7589387427737242</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -525,7 +525,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.837336513612047</v>
+        <v>1.830845269518987</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -541,7 +541,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>911.792313465562</v>
+        <v>914.0617569498547</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -549,7 +549,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.996914479034826</v>
+        <v>0.9547297179517178</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -557,7 +557,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1.043603957184384</v>
+        <v>0.9393391234223979</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -565,7 +565,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2.438318679536144</v>
+        <v>2.438758919211486</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -573,7 +573,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.9143124230210719</v>
+        <v>0.914490606252917</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -581,7 +581,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.07861273110841929</v>
+        <v>0.07821515985127751</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -605,7 +605,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.4514699659210243</v>
+        <v>0.4594743153861449</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -613,7 +613,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.1240976608660041</v>
+        <v>0.1275017474602679</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -621,7 +621,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.1261334473710915</v>
+        <v>0.1265271498996089</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -629,7 +629,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>5.111223875363915</v>
+        <v>5.107268771530819</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -637,7 +637,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.02398805754537087</v>
+        <v>0.2382463473900343</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -645,7 +645,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.4025288533106691</v>
+        <v>0.4067438140266562</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -653,7 +653,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>28.30953480000747</v>
+        <v>28.30467215265686</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -661,7 +661,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>29.29989211099639</v>
+        <v>29.29985665220562</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -669,7 +669,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.08197672604051731</v>
+        <v>0.08220955371778636</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -677,7 +677,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.4545313486121543</v>
+        <v>0.4548255380773952</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -685,7 +685,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1.705194716364508</v>
+        <v>1.708027906264028</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -693,7 +693,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>3.598839880666221</v>
+        <v>3.595510537878962</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -701,7 +701,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>12.06553132622813</v>
+        <v>12.06648340382061</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -709,7 +709,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>33.13895501724645</v>
+        <v>33.16550990136131</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -717,7 +717,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>73837.95399240138</v>
+        <v>73852.54308902436</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -725,7 +725,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>9.003384068945799</v>
+        <v>9.001542361301979</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -733,7 +733,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>88.20035389461961</v>
+        <v>87.63091361475982</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -741,7 +741,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>135.3840187081974</v>
+        <v>152.2856605377513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   MonteCarlo_Sim.py 	modified:   Tools.py
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_inputs.xlsx
+++ b/Outputs/MonteCarlo_sim_inputs.xlsx
@@ -472,10 +472,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.07840549344390262</v>
+        <v>0.07844425225260536</v>
       </c>
       <c r="C2">
-        <v>0.07862291976524574</v>
+        <v>0.0782501778507621</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -483,10 +483,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>23.13926674507044</v>
+        <v>23.13902426738357</v>
       </c>
       <c r="C3">
-        <v>23.13772295332353</v>
+        <v>23.13854921214313</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -494,10 +494,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>151.7000267548202</v>
+        <v>151.7000087709266</v>
       </c>
       <c r="C4">
-        <v>151.700136362501</v>
+        <v>151.7000486805258</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -505,10 +505,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.186380695526576</v>
+        <v>0.1859816921622611</v>
       </c>
       <c r="C5">
-        <v>0.1859380895574332</v>
+        <v>0.1857631005249513</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -516,10 +516,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.549961672622671</v>
+        <v>2.549980640079351</v>
       </c>
       <c r="C6">
-        <v>2.550004618182619</v>
+        <v>2.550019590994558</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -527,10 +527,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.766278500269526</v>
+        <v>0.7692259974068437</v>
       </c>
       <c r="C7">
-        <v>0.7609507999723486</v>
+        <v>0.7631674057556723</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -549,10 +549,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.824138351953377</v>
+        <v>1.825554439925985</v>
       </c>
       <c r="C9">
-        <v>1.83857571564826</v>
+        <v>1.824893393937746</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -571,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>914.9678682306077</v>
+        <v>907.4136508152212</v>
       </c>
       <c r="C11">
-        <v>916.7986329393781</v>
+        <v>910.2021873357731</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -582,10 +582,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.9706576401783353</v>
+        <v>0.9749011072409366</v>
       </c>
       <c r="C12">
-        <v>1.013146883615496</v>
+        <v>1.075446053817627</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -593,10 +593,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1.050826187909775</v>
+        <v>0.9402340008544148</v>
       </c>
       <c r="C13">
-        <v>0.9100805038813456</v>
+        <v>0.9951654437442093</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -604,10 +604,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2.438473708641736</v>
+        <v>2.438056001776486</v>
       </c>
       <c r="C14">
-        <v>2.4384699261776</v>
+        <v>2.438471660727712</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -615,10 +615,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.9143730062035123</v>
+        <v>0.9142119329940921</v>
       </c>
       <c r="C15">
-        <v>0.9142128036552708</v>
+        <v>0.914256720186948</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -626,10 +626,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.07868960042828718</v>
+        <v>0.07815659036814897</v>
       </c>
       <c r="C16">
-        <v>0.07824633705419502</v>
+        <v>0.07882760274675904</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -659,10 +659,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.457726872674761</v>
+        <v>0.4549029917249756</v>
       </c>
       <c r="C19">
-        <v>0.4599561130293039</v>
+        <v>0.4536924731850582</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -670,10 +670,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.1302621020758346</v>
+        <v>0.1259456542906707</v>
       </c>
       <c r="C20">
-        <v>0.1261775939791664</v>
+        <v>0.1269705784710714</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -681,10 +681,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.1265644202156551</v>
+        <v>0.1288642172820511</v>
       </c>
       <c r="C21">
-        <v>0.1252756897915584</v>
+        <v>0.1252681519406583</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -692,10 +692,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>5.109355790632157</v>
+        <v>5.109687419198908</v>
       </c>
       <c r="C22">
-        <v>5.112203921094046</v>
+        <v>5.10790859792463</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -703,10 +703,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-0.00137290989612285</v>
+        <v>-0.004097353059522491</v>
       </c>
       <c r="C23">
-        <v>-0.1423578906310613</v>
+        <v>0.00804272403612475</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -714,10 +714,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.4058646342157485</v>
+        <v>0.4033872098114001</v>
       </c>
       <c r="C24">
-        <v>0.4025843713677514</v>
+        <v>0.4056507790300997</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -725,10 +725,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>28.30473808899301</v>
+        <v>28.30654607309969</v>
       </c>
       <c r="C25">
-        <v>28.30545395994884</v>
+        <v>28.30365333274037</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -736,10 +736,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>29.29996561896763</v>
+        <v>29.29958102108359</v>
       </c>
       <c r="C26">
-        <v>29.30042924278149</v>
+        <v>29.29978708603336</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -747,10 +747,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.08154067457270446</v>
+        <v>0.08189844844316098</v>
       </c>
       <c r="C27">
-        <v>0.08181696289040449</v>
+        <v>0.08213406191251332</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -758,10 +758,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.4550525709669269</v>
+        <v>0.4546600195179318</v>
       </c>
       <c r="C28">
-        <v>0.4547690901704541</v>
+        <v>0.4544837018245149</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -769,10 +769,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1.707059273072075</v>
+        <v>1.70654392870338</v>
       </c>
       <c r="C29">
-        <v>1.70696300185747</v>
+        <v>1.706871611059007</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -780,10 +780,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>3.598644448864434</v>
+        <v>3.598086841575389</v>
       </c>
       <c r="C30">
-        <v>3.59524334656172</v>
+        <v>3.596349917560963</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -791,10 +791,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>12.06433373095802</v>
+        <v>12.06547291340627</v>
       </c>
       <c r="C31">
-        <v>12.06589706912847</v>
+        <v>12.0654267495494</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -802,10 +802,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>33.96553020092333</v>
+        <v>33.39448477844254</v>
       </c>
       <c r="C32">
-        <v>34.18858763833033</v>
+        <v>33.37300287709702</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -813,10 +813,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>73825.69322420191</v>
+        <v>73843.24066627219</v>
       </c>
       <c r="C33">
-        <v>73824.97433838586</v>
+        <v>73797.24431837903</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -824,10 +824,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>9.000681356505888</v>
+        <v>9.004229623816084</v>
       </c>
       <c r="C34">
-        <v>9.001685133517118</v>
+        <v>8.999396750164943</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -835,10 +835,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>88.12115968413913</v>
+        <v>87.55305656026985</v>
       </c>
       <c r="C35">
-        <v>88.43815689630055</v>
+        <v>87.95448089355044</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -846,10 +846,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>180.3978277516457</v>
+        <v>124.2173221769794</v>
       </c>
       <c r="C36">
-        <v>141.3391787714986</v>
+        <v>122.8319242020687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   MonteCarlo_Data_Analysis.py 	modified:   MonteCarlo_Sim.py 	modified:   Outputs/MonteCarlo_sim_inputs.xlsx 	modified:   Outputs/MonteCarlo_sim_outputs.xlsx 	modified:   Outputs/MonteCarlo_sim_wind.xlsx 	modified:   Tools.py
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_inputs.xlsx
+++ b/Outputs/MonteCarlo_sim_inputs.xlsx
@@ -472,10 +472,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.07844425225260536</v>
+        <v>0.07881312460784126</v>
       </c>
       <c r="C2">
-        <v>0.0782501778507621</v>
+        <v>0.07868058796995309</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -483,10 +483,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>23.13902426738357</v>
+        <v>23.13921682692138</v>
       </c>
       <c r="C3">
-        <v>23.13854921214313</v>
+        <v>23.13993403873709</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -494,10 +494,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>151.7000087709266</v>
+        <v>151.7001364441091</v>
       </c>
       <c r="C4">
-        <v>151.7000486805258</v>
+        <v>151.7000501335764</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -505,10 +505,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1859816921622611</v>
+        <v>0.1858915563524067</v>
       </c>
       <c r="C5">
-        <v>0.1857631005249513</v>
+        <v>0.1860573123609745</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -516,10 +516,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.549980640079351</v>
+        <v>2.550002061758742</v>
       </c>
       <c r="C6">
-        <v>2.550019590994558</v>
+        <v>2.549960751924217</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -527,10 +527,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.7692259974068437</v>
+        <v>0.7718942589664032</v>
       </c>
       <c r="C7">
-        <v>0.7631674057556723</v>
+        <v>0.7619561242120835</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -549,10 +549,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.825554439925985</v>
+        <v>1.827249818929199</v>
       </c>
       <c r="C9">
-        <v>1.824893393937746</v>
+        <v>1.832533843157625</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -571,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>907.4136508152212</v>
+        <v>917.7353696920507</v>
       </c>
       <c r="C11">
-        <v>910.2021873357731</v>
+        <v>916.3224302482407</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -582,10 +582,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.9749011072409366</v>
+        <v>0.9923146550803537</v>
       </c>
       <c r="C12">
-        <v>1.075446053817627</v>
+        <v>0.99013189318705</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -593,10 +593,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.9402340008544148</v>
+        <v>1.052976498902757</v>
       </c>
       <c r="C13">
-        <v>0.9951654437442093</v>
+        <v>0.9580825004213104</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -604,10 +604,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2.438056001776486</v>
+        <v>2.438337820041923</v>
       </c>
       <c r="C14">
-        <v>2.438471660727712</v>
+        <v>2.438558578626186</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -615,10 +615,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.9142119329940921</v>
+        <v>0.9145347591184037</v>
       </c>
       <c r="C15">
-        <v>0.914256720186948</v>
+        <v>0.9142978354870943</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -626,10 +626,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.07815659036814897</v>
+        <v>0.07859319507629441</v>
       </c>
       <c r="C16">
-        <v>0.07882760274675904</v>
+        <v>0.07861429794597517</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -659,10 +659,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.4549029917249756</v>
+        <v>0.4584993047979745</v>
       </c>
       <c r="C19">
-        <v>0.4536924731850582</v>
+        <v>0.4519771706760511</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -670,10 +670,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.1259456542906707</v>
+        <v>0.1304844436502391</v>
       </c>
       <c r="C20">
-        <v>0.1269705784710714</v>
+        <v>0.1232399248041299</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -681,10 +681,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.1288642172820511</v>
+        <v>0.1291677274760185</v>
       </c>
       <c r="C21">
-        <v>0.1252681519406583</v>
+        <v>0.1263881077842832</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -692,10 +692,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>5.109687419198908</v>
+        <v>5.104926529470156</v>
       </c>
       <c r="C22">
-        <v>5.10790859792463</v>
+        <v>5.10987551632889</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -703,10 +703,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-0.004097353059522491</v>
+        <v>-0.0242139505116133</v>
       </c>
       <c r="C23">
-        <v>0.00804272403612475</v>
+        <v>0.00503156547321891</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -714,10 +714,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.4033872098114001</v>
+        <v>0.4089624395380318</v>
       </c>
       <c r="C24">
-        <v>0.4056507790300997</v>
+        <v>0.4042404135919265</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -725,10 +725,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>28.30654607309969</v>
+        <v>28.30648952303393</v>
       </c>
       <c r="C25">
-        <v>28.30365333274037</v>
+        <v>28.30598363412188</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -736,10 +736,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>29.29958102108359</v>
+        <v>29.29966712599418</v>
       </c>
       <c r="C26">
-        <v>29.29978708603336</v>
+        <v>29.29963692361504</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -747,10 +747,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.08189844844316098</v>
+        <v>0.08208752150269018</v>
       </c>
       <c r="C27">
-        <v>0.08213406191251332</v>
+        <v>0.08204491330088279</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -758,10 +758,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.4546600195179318</v>
+        <v>0.4543619591828427</v>
       </c>
       <c r="C28">
-        <v>0.4544837018245149</v>
+        <v>0.4543825076948632</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -769,10 +769,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1.70654392870338</v>
+        <v>1.707315648853719</v>
       </c>
       <c r="C29">
-        <v>1.706871611059007</v>
+        <v>1.706783468221732</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -780,10 +780,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>3.598086841575389</v>
+        <v>3.597811388646879</v>
       </c>
       <c r="C30">
-        <v>3.596349917560963</v>
+        <v>3.596831469393622</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -791,10 +791,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>12.06547291340627</v>
+        <v>12.06603796442994</v>
       </c>
       <c r="C31">
-        <v>12.0654267495494</v>
+        <v>12.06554974753924</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -802,10 +802,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>33.39448477844254</v>
+        <v>33.41805094524368</v>
       </c>
       <c r="C32">
-        <v>33.37300287709702</v>
+        <v>33.13508559218115</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -813,10 +813,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>73843.24066627219</v>
+        <v>73866.9865992866</v>
       </c>
       <c r="C33">
-        <v>73797.24431837903</v>
+        <v>73852.06545373233</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -824,10 +824,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>9.004229623816084</v>
+        <v>9.003243897527003</v>
       </c>
       <c r="C34">
-        <v>8.999396750164943</v>
+        <v>9.007231799129405</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -835,10 +835,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>87.55305656026985</v>
+        <v>88.06246075798238</v>
       </c>
       <c r="C35">
-        <v>87.95448089355044</v>
+        <v>87.88212135037369</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -846,10 +846,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>124.2173221769794</v>
+        <v>142.7725302575142</v>
       </c>
       <c r="C36">
-        <v>122.8319242020687</v>
+        <v>90.42901659229462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>